<commit_message>
fix. narration auto skip
</commit_message>
<xml_diff>
--- a/WhiteCane/Assets/Resources/Xlsx/SoundData.xlsx
+++ b/WhiteCane/Assets/Resources/Xlsx/SoundData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,15 +42,25 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>intro_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intro_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intro_02</t>
+    <t>tutorial02</t>
+  </si>
+  <si>
+    <t>tutorial03</t>
+  </si>
+  <si>
+    <t>tutorial04</t>
+  </si>
+  <si>
+    <t>tutorial05</t>
+  </si>
+  <si>
+    <t>tutorial06</t>
+  </si>
+  <si>
+    <t>tutorial07</t>
+  </si>
+  <si>
+    <t>tutorial08</t>
   </si>
   <si>
     <t>tutorial01</t>
@@ -61,85 +71,120 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tutorial02</t>
-  </si>
-  <si>
-    <t>tutorial03</t>
-  </si>
-  <si>
-    <t>tutorial04</t>
-  </si>
-  <si>
-    <t>tutorial05</t>
-  </si>
-  <si>
-    <t>tutorial06</t>
-  </si>
-  <si>
-    <t>tutorial07</t>
-  </si>
-  <si>
-    <t>tutorial08</t>
-  </si>
-  <si>
-    <t>tutorial09</t>
+    <t>Lysoniastep01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tutorial09</t>
+    <t>Lysoniastep02</t>
+  </si>
+  <si>
+    <t>Lysoniastep03</t>
+  </si>
+  <si>
+    <t>Lysoniastep04</t>
+  </si>
+  <si>
+    <t>Lysoniastep05</t>
+  </si>
+  <si>
+    <t>Lysoniastep06</t>
+  </si>
+  <si>
+    <t>Lysoniastep07</t>
+  </si>
+  <si>
+    <t>Lysoniastep08</t>
+  </si>
+  <si>
+    <t>Lysoniastep09</t>
+  </si>
+  <si>
+    <t>Lysoniastep10</t>
+  </si>
+  <si>
+    <t>Lysoniastep11</t>
+  </si>
+  <si>
+    <t>Lysoniastep12</t>
+  </si>
+  <si>
+    <t>Lysoniastep13</t>
+  </si>
+  <si>
+    <t>Lysoniastep14</t>
+  </si>
+  <si>
+    <t>Lysoniastep15</t>
+  </si>
+  <si>
+    <t>Lysoniastep16</t>
+  </si>
+  <si>
+    <t>Lysoniastep17</t>
+  </si>
+  <si>
+    <t>Lysoniastep18</t>
+  </si>
+  <si>
+    <t>Lysoniastep19</t>
+  </si>
+  <si>
+    <t>Lysoniastep20</t>
+  </si>
+  <si>
+    <t>Lysoniastep21</t>
+  </si>
+  <si>
+    <t>Lysoniastep22</t>
+  </si>
+  <si>
+    <t>Lysoniastep23</t>
+  </si>
+  <si>
+    <t>Lysoniastep24</t>
+  </si>
+  <si>
+    <t>Lysoniastep25</t>
+  </si>
+  <si>
+    <t>Lysoniastep26</t>
+  </si>
+  <si>
+    <t>Lysoniastep27</t>
+  </si>
+  <si>
+    <t>Lysoniastep28</t>
+  </si>
+  <si>
+    <t>Lysoniastep29</t>
+  </si>
+  <si>
+    <t>Lysoniastep30</t>
+  </si>
+  <si>
+    <t>Lysoniastep31</t>
+  </si>
+  <si>
+    <t>Lysoniastep32</t>
+  </si>
+  <si>
+    <t>Lysoniastep33</t>
+  </si>
+  <si>
+    <t>Lysoniastep34</t>
+  </si>
+  <si>
+    <t>Lysoniastep35</t>
+  </si>
+  <si>
+    <t>Lysoniastep36</t>
+  </si>
+  <si>
+    <t>Lysoniastep37</t>
+  </si>
+  <si>
+    <t>Lysoniastep01</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tutorial10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tutorial10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreset_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreset_02</t>
-  </si>
-  <si>
-    <t>foreset_03</t>
-  </si>
-  <si>
-    <t>foreset_04</t>
-  </si>
-  <si>
-    <t>foreset_05</t>
-  </si>
-  <si>
-    <t>foreset_06</t>
-  </si>
-  <si>
-    <t>foreset_07</t>
-  </si>
-  <si>
-    <t>foreset_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreset_07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreset_08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreset_09</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>foreset_08</t>
-  </si>
-  <si>
-    <t>foreset_09</t>
   </si>
 </sst>
 </file>
@@ -480,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -516,171 +561,363 @@
     </row>
     <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
-        <v>30</v>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>